<commit_message>
Fixed heat flow nomenclature.
</commit_message>
<xml_diff>
--- a/docs/MARVEL Thermal components.xlsx
+++ b/docs/MARVEL Thermal components.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\hkn21281\PycharmProjects\Thermal\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\hkn21281\PycharmProjects\thermal\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57AE46D7-C2D6-4DEE-BA80-BE16A70A88A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D96F81-8FBE-4983-8EDF-BE2AA69AC667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{42DAC784-73B3-45B2-A410-D7F9E3ED47F6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{42DAC784-73B3-45B2-A410-D7F9E3ED47F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -241,8 +241,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8191500" y="1952625"/>
-          <a:ext cx="7153275" cy="4305300"/>
+          <a:off x="9396693" y="2102037"/>
+          <a:ext cx="7186145" cy="4223123"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2199,17 +2199,17 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y25" sqref="Y25"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5546875" customWidth="1"/>
+    <col min="2" max="2" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>27428</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>41091</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>72048</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>52768</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>163143</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2328,7 +2328,7 @@
         <v>7012</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>0.34300000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -2364,7 +2364,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>24</v>
       </c>

</xml_diff>